<commit_message>
Updated description of BFR 2019, adjusted sectors of Skidpad and fixed a potential small bug in openlap for single point tracks
</commit_message>
<xml_diff>
--- a/BFR 2019.xlsx
+++ b/BFR 2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solon\Documents\MATLAB\OpenLAP-Lap-Time-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA711711-5030-455B-881F-B734227DBC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E7C2D6-24B3-4E7A-BFDA-FEDFB02EE343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -345,12 +345,6 @@
     <t>From crancskaft to Input shaft.</t>
   </si>
   <si>
-    <t>BFR 2021</t>
-  </si>
-  <si>
-    <t>Brown Formula Racing 2021 Car</t>
-  </si>
-  <si>
     <t>[Steering Wheel Angle]/[Wheel Angle] (src: Spec Sheet 2019)</t>
   </si>
   <si>
@@ -406,6 +400,12 @@
   </si>
   <si>
     <t>From m1 tune package on 5/4/2019, I think this was the timing we used for competition. This number could be lower for the future/improved cars</t>
+  </si>
+  <si>
+    <t>BFR 2019</t>
+  </si>
+  <si>
+    <t>Brown Formula Racing 2019 Car</t>
   </si>
 </sst>
 </file>
@@ -1095,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1126,10 +1126,10 @@
         <v>49</v>
       </c>
       <c r="F1" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G1" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1140,13 +1140,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1178,10 +1178,10 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1197,10 +1197,10 @@
       </c>
       <c r="E5" s="15"/>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1218,10 +1218,10 @@
       </c>
       <c r="E6" s="20"/>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1238,13 +1238,13 @@
         <v>38</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1264,10 +1264,10 @@
         <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1285,10 +1285,10 @@
         <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1495,10 +1495,10 @@
         <v>87</v>
       </c>
       <c r="F23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1513,7 +1513,7 @@
         <v>38</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1576,10 +1576,10 @@
         <v>88</v>
       </c>
       <c r="F28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1597,10 +1597,10 @@
         <v>89</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1618,10 +1618,10 @@
         <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1639,10 +1639,10 @@
         <v>91</v>
       </c>
       <c r="F31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G31" t="s">
         <v>105</v>
-      </c>
-      <c r="G31" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
@@ -1660,10 +1660,10 @@
         <v>91</v>
       </c>
       <c r="F32" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" t="s">
         <v>105</v>
-      </c>
-      <c r="G32" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1711,10 +1711,10 @@
         <v>93</v>
       </c>
       <c r="F35" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G35" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1747,10 +1747,10 @@
         <v>80</v>
       </c>
       <c r="F37" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G37" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1813,10 +1813,10 @@
         <v>96</v>
       </c>
       <c r="F41" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" t="s">
         <v>110</v>
-      </c>
-      <c r="G41" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1832,10 +1832,10 @@
       </c>
       <c r="E42" s="21"/>
       <c r="F42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G42" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1851,10 +1851,10 @@
       </c>
       <c r="E43" s="21"/>
       <c r="F43" t="s">
+        <v>108</v>
+      </c>
+      <c r="G43" t="s">
         <v>110</v>
-      </c>
-      <c r="G43" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1870,10 +1870,10 @@
       </c>
       <c r="E44" s="21"/>
       <c r="F44" t="s">
+        <v>108</v>
+      </c>
+      <c r="G44" t="s">
         <v>110</v>
-      </c>
-      <c r="G44" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1889,10 +1889,10 @@
       </c>
       <c r="E45" s="21"/>
       <c r="F45" t="s">
+        <v>108</v>
+      </c>
+      <c r="G45" t="s">
         <v>110</v>
-      </c>
-      <c r="G45" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1908,10 +1908,10 @@
       </c>
       <c r="E46" s="21"/>
       <c r="F46" t="s">
+        <v>108</v>
+      </c>
+      <c r="G46" t="s">
         <v>110</v>
-      </c>
-      <c r="G46" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1927,10 +1927,10 @@
       </c>
       <c r="E47" s="21"/>
       <c r="F47" t="s">
+        <v>108</v>
+      </c>
+      <c r="G47" t="s">
         <v>110</v>
-      </c>
-      <c r="G47" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1946,10 +1946,10 @@
       </c>
       <c r="E48" s="21"/>
       <c r="F48" t="s">
+        <v>108</v>
+      </c>
+      <c r="G48" t="s">
         <v>110</v>
-      </c>
-      <c r="G48" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -1963,10 +1963,10 @@
       </c>
       <c r="E49" s="21"/>
       <c r="F49" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G49" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2040,10 +2040,10 @@
         <v>16</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2054,10 +2054,10 @@
         <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2068,7 +2068,7 @@
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
More accurate tire data
</commit_message>
<xml_diff>
--- a/BFR 2019.xlsx
+++ b/BFR 2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Solon\Documents\MATLAB\OpenLAP-Lap-Time-Simulator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob Morse\Documents\Car Data\OpenLAP-Lap-Time-Simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E7C2D6-24B3-4E7A-BFDA-FEDFB02EE343}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C41308D-4871-48A9-9A35-BF5323A85EAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="15196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
   <si>
     <t>General</t>
   </si>
@@ -406,6 +406,9 @@
   </si>
   <si>
     <t>Brown Formula Racing 2019 Car</t>
+  </si>
+  <si>
+    <t>JM, 6/4/20</t>
   </si>
 </sst>
 </file>
@@ -1095,21 +1098,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5234375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.1015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.05078125" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.06640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="23" t="s">
         <v>45</v>
       </c>
@@ -1132,7 +1135,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="34" t="s">
         <v>0</v>
       </c>
@@ -1149,7 +1152,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="35"/>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1162,7 +1165,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="34" t="s">
         <v>12</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="35"/>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -1203,7 +1206,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="16" t="s">
         <v>10</v>
       </c>
@@ -1224,7 +1227,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="16" t="s">
         <v>11</v>
       </c>
@@ -1247,7 +1250,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="34" t="s">
         <v>14</v>
       </c>
@@ -1270,7 +1273,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="36"/>
       <c r="B9" s="2" t="s">
         <v>73</v>
@@ -1291,7 +1294,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="36"/>
       <c r="B10" s="2" t="s">
         <v>21</v>
@@ -1304,7 +1307,7 @@
       </c>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="36"/>
       <c r="B11" s="2" t="s">
         <v>22</v>
@@ -1317,7 +1320,7 @@
       </c>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="36"/>
       <c r="B12" s="2" t="s">
         <v>71</v>
@@ -1330,7 +1333,7 @@
       </c>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="36"/>
       <c r="B13" s="2" t="s">
         <v>17</v>
@@ -1343,7 +1346,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="35"/>
       <c r="B14" s="12" t="s">
         <v>23</v>
@@ -1358,7 +1361,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="34" t="s">
         <v>20</v>
       </c>
@@ -1375,7 +1378,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="36"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
@@ -1390,7 +1393,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="36"/>
       <c r="B17" s="2" t="s">
         <v>77</v>
@@ -1405,7 +1408,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="36"/>
       <c r="B18" s="2" t="s">
         <v>26</v>
@@ -1420,7 +1423,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="36"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
@@ -1435,7 +1438,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="36"/>
       <c r="B20" s="2" t="s">
         <v>28</v>
@@ -1450,7 +1453,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="35"/>
       <c r="B21" s="12" t="s">
         <v>29</v>
@@ -1465,7 +1468,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="34" t="s">
         <v>30</v>
       </c>
@@ -1480,7 +1483,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="36"/>
       <c r="B23" s="2" t="s">
         <v>31</v>
@@ -1501,7 +1504,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="36"/>
       <c r="B24" s="2" t="s">
         <v>36</v>
@@ -1516,7 +1519,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="36"/>
       <c r="B25" s="2" t="s">
         <v>32</v>
@@ -1531,7 +1534,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="36"/>
       <c r="B26" s="2" t="s">
         <v>33</v>
@@ -1546,7 +1549,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="36"/>
       <c r="B27" s="2" t="s">
         <v>34</v>
@@ -1561,13 +1564,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="36"/>
       <c r="B28" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C28" s="4">
-        <v>2.0684</v>
+        <v>1.7201</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>38</v>
@@ -1576,13 +1579,13 @@
         <v>88</v>
       </c>
       <c r="F28" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="G28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="36"/>
       <c r="B29" s="2" t="s">
         <v>40</v>
@@ -1603,13 +1606,13 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="36"/>
       <c r="B30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C30" s="4">
-        <v>3.8900000000000002E-4</v>
+        <v>3.3473999999999998E-4</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>35</v>
@@ -1618,13 +1621,13 @@
         <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="G30" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="36"/>
       <c r="B31" s="2" t="s">
         <v>42</v>
@@ -1645,7 +1648,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A32" s="35"/>
       <c r="B32" s="12" t="s">
         <v>43</v>
@@ -1666,7 +1669,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="34" t="s">
         <v>50</v>
       </c>
@@ -1681,7 +1684,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="36"/>
       <c r="B34" s="2" t="s">
         <v>52</v>
@@ -1696,7 +1699,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A35" s="35"/>
       <c r="B35" s="12" t="s">
         <v>53</v>
@@ -1717,7 +1720,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="31" t="s">
         <v>55</v>
       </c>
@@ -1732,7 +1735,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="32"/>
       <c r="B37" s="5" t="s">
         <v>78</v>
@@ -1753,7 +1756,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="32"/>
       <c r="B38" s="5" t="s">
         <v>74</v>
@@ -1768,7 +1771,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="32"/>
       <c r="B39" s="5" t="s">
         <v>75</v>
@@ -1783,7 +1786,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="32"/>
       <c r="B40" s="5" t="s">
         <v>76</v>
@@ -1798,7 +1801,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="32"/>
       <c r="B41" s="2" t="s">
         <v>59</v>
@@ -1819,7 +1822,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="32"/>
       <c r="B42" s="2" t="s">
         <v>60</v>
@@ -1838,7 +1841,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="32"/>
       <c r="B43" s="27" t="s">
         <v>61</v>
@@ -1857,7 +1860,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="32"/>
       <c r="B44" s="27" t="s">
         <v>62</v>
@@ -1876,7 +1879,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="32"/>
       <c r="B45" s="27" t="s">
         <v>63</v>
@@ -1895,7 +1898,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="32"/>
       <c r="B46" s="27" t="s">
         <v>64</v>
@@ -1914,7 +1917,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="32"/>
       <c r="B47" s="27" t="s">
         <v>65</v>
@@ -1933,7 +1936,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="32"/>
       <c r="B48" s="27" t="s">
         <v>66</v>
@@ -1952,7 +1955,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="32"/>
       <c r="B49" s="27" t="s">
         <v>67</v>
@@ -1969,7 +1972,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="32"/>
       <c r="B50" s="27" t="s">
         <v>68</v>
@@ -1980,7 +1983,7 @@
       </c>
       <c r="E50" s="21"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="32"/>
       <c r="B51" s="27" t="s">
         <v>69</v>
@@ -1991,7 +1994,7 @@
       </c>
       <c r="E51" s="21"/>
     </row>
-    <row r="52" spans="1:7" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A52" s="33"/>
       <c r="B52" s="28" t="s">
         <v>70</v>
@@ -2026,13 +2029,13 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -2046,7 +2049,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3000</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4000</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5000</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>6000</v>
       </c>
@@ -2103,7 +2106,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>7000</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>7175.3992173522829</v>
       </c>
@@ -2119,7 +2122,7 @@
         <v>35.182831953706831</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>7506.1153287687093</v>
       </c>
@@ -2127,7 +2130,7 @@
         <v>36.847512136620168</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>8007.8914978143248</v>
       </c>
@@ -2135,7 +2138,7 @@
         <v>37.941984775920879</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>8511.9484676283282</v>
       </c>
@@ -2143,7 +2146,7 @@
         <v>43.916460499061756</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>9002.3206328319975</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>46.388591342763647</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>9510.9392041827778</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>45.079431223908209</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
         <v>10005.872970923225</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>42.509137210022118</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>10500.80673766367</v>
       </c>
@@ -2175,7 +2178,7 @@
         <v>39.0591714577223</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>11000.302105940895</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>35.162916343343291</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>11508.920677291677</v>
       </c>
@@ -2191,7 +2194,7 @@
         <v>31.826747597300376</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>12001.573643263735</v>
       </c>
@@ -2199,7 +2202,7 @@
         <v>28.840817002649366</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>12507.911413846128</v>
       </c>
@@ -2207,7 +2210,7 @@
         <v>25.420624467082625</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>12902.489946777452</v>
       </c>

</xml_diff>